<commit_message>
"Working Code until Number of maximum matches"
</commit_message>
<xml_diff>
--- a/imbp.xlsx
+++ b/imbp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adharvan/PycharmProjects/ConvoPartners/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B377182-C859-5644-A3CA-E3063A8D5F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BD90A4-611C-3B48-B316-D90D2A8717DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DC7B3BA4-3156-1747-B52E-D36301AD8978}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="545">
   <si>
     <t>Training Timestamp</t>
   </si>
@@ -2047,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D501316-0379-AC4F-A612-885024FB02A8}">
   <dimension ref="A1:X1220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2062,6 +2062,7 @@
     <col min="7" max="7" width="34.5" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
     <col min="12" max="12" width="25.6640625" customWidth="1"/>
+    <col min="13" max="13" width="53.33203125" customWidth="1"/>
     <col min="19" max="19" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2210,9 +2211,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>

</xml_diff>